<commit_message>
right graph for inception 1gbps, in rack, uneven, striping
</commit_message>
<xml_diff>
--- a/distributed-tensorflow-simulator/exp_results/inception-v3/graphs/1gbps_inrack_uneven_striping.xlsx
+++ b/distributed-tensorflow-simulator/exp_results/inception-v3/graphs/1gbps_inrack_uneven_striping.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -261,19 +258,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.8017</c:v>
+                    <c:v>1.2476</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.5631</c:v>
+                    <c:v>0.9011</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.91</c:v>
+                    <c:v>0.7133</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.0961</c:v>
+                    <c:v>0.3268</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2912</c:v>
+                    <c:v>0.3421</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -285,19 +282,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.9308</c:v>
+                    <c:v>0.8028</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.3955</c:v>
+                    <c:v>1.1751</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.5383</c:v>
+                    <c:v>1.4831</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.0137</c:v>
+                    <c:v>0.9313</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3249</c:v>
+                    <c:v>0.6935</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -350,16 +347,16 @@
                   <c:v>19.1621</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.6127</c:v>
+                  <c:v>31.4453</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.8396</c:v>
+                  <c:v>37.3278</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.1408</c:v>
+                  <c:v>40.4457</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.9243</c:v>
+                  <c:v>42.1045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -408,19 +405,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.5409</c:v>
+                    <c:v>1.5588</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.4896</c:v>
+                    <c:v>1.1747</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1917</c:v>
+                    <c:v>0.1055</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.6268</c:v>
+                    <c:v>1.152</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.9901</c:v>
+                    <c:v>0.5039</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -432,19 +429,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1679</c:v>
+                    <c:v>0.1526</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0021</c:v>
+                    <c:v>0.0016</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.0932</c:v>
+                    <c:v>1.3906</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.6782</c:v>
+                    <c:v>0.7429</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.7769</c:v>
+                    <c:v>0.2732</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -494,19 +491,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>19.7154</c:v>
+                  <c:v>19.6975</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>31.9728</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.4174</c:v>
+                  <c:v>38.5036</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.2563</c:v>
+                  <c:v>41.4647</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42.8794</c:v>
+                  <c:v>43.2215</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,19 +552,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.2933</c:v>
+                    <c:v>1.0842</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.3297</c:v>
+                    <c:v>2.548</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.2372</c:v>
+                    <c:v>2.3476</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2039</c:v>
+                    <c:v>1.8071</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1415</c:v>
+                    <c:v>1.0542</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -579,19 +576,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>2.8994</c:v>
+                    <c:v>2.1093</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0021</c:v>
+                    <c:v>0.0076</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>1.9424</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.8247</c:v>
+                    <c:v>1.3339</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2506</c:v>
+                    <c:v>2.4016</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -641,7 +638,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12.691</c:v>
+                  <c:v>11.8906</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>25.2292</c:v>
@@ -650,10 +647,10 @@
                   <c:v>35.0064</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.8738</c:v>
+                  <c:v>40.4233</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44.3616</c:v>
+                  <c:v>43.3887</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,19 +699,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.9418</c:v>
+                    <c:v>0.434</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.061</c:v>
+                    <c:v>2.7386</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>1.1856</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.4012</c:v>
+                    <c:v>0.5249</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.9584</c:v>
+                    <c:v>0.6442</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -726,19 +723,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.1822</c:v>
+                    <c:v>1.032</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1504</c:v>
+                    <c:v>0.305</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.5912</c:v>
+                    <c:v>1.6113</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.9242</c:v>
+                    <c:v>2.515</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2077</c:v>
+                    <c:v>1.0473</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -788,19 +785,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.5906</c:v>
+                  <c:v>0.8386</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.4313</c:v>
+                  <c:v>13.4507</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24.8925</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.9184</c:v>
+                  <c:v>35.2796</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.2117</c:v>
+                  <c:v>40.7455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,11 +812,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2104983024"/>
-        <c:axId val="-2055803328"/>
+        <c:axId val="-2071671072"/>
+        <c:axId val="-2071663040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2104983024"/>
+        <c:axId val="-2071671072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -936,12 +933,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2055803328"/>
+        <c:crossAx val="-2071663040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2055803328"/>
+        <c:axId val="-2071663040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2104983024"/>
+        <c:crossAx val="-2071671072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1293,19 +1290,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0084</c:v>
+                    <c:v>0.5764</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0183</c:v>
+                    <c:v>0.4101</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.416</c:v>
+                    <c:v>1.0938</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.1206</c:v>
+                    <c:v>1.6701</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.6765</c:v>
+                    <c:v>0.8139</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1317,19 +1314,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.048</c:v>
+                    <c:v>1.0596</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.4162</c:v>
+                    <c:v>0.8295</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.9084</c:v>
+                    <c:v>0.6738</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2837</c:v>
+                    <c:v>1.3469</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5374</c:v>
+                    <c:v>0.9206</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1379,19 +1376,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>25.0944</c:v>
+                  <c:v>25.1028</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.7742</c:v>
+                  <c:v>37.782</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44.4965</c:v>
+                  <c:v>44.383</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.9898</c:v>
+                  <c:v>47.4391</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.8374</c:v>
+                  <c:v>49.0667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,19 +1437,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0112</c:v>
+                    <c:v>0.0023</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0009</c:v>
+                    <c:v>0.4246</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.526</c:v>
+                    <c:v>1.1014</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.451</c:v>
+                    <c:v>0.9892</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.8385</c:v>
+                    <c:v>0.9141</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1464,19 +1461,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.0956</c:v>
+                    <c:v>1.1045</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.4215</c:v>
+                    <c:v>0.8362</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>0.7956</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.1124</c:v>
+                    <c:v>0.8953</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.4209</c:v>
+                    <c:v>0.9062</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1526,7 +1523,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>27.6744</c:v>
+                  <c:v>27.6833</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>41.154</c:v>
@@ -1535,10 +1532,10 @@
                   <c:v>48.0364</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51.3833</c:v>
+                  <c:v>51.0812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53.1588</c:v>
+                  <c:v>52.9243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,19 +1584,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.0049</c:v>
+                    <c:v>1.1493</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.002</c:v>
+                    <c:v>0.5001</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.223</c:v>
+                    <c:v>1.6391</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.5079</c:v>
+                    <c:v>4.8859</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.724</c:v>
+                    <c:v>1.7432</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1611,19 +1608,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1364</c:v>
+                    <c:v>0.0757</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.5105</c:v>
+                    <c:v>0.9624</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0014</c:v>
+                    <c:v>0.7157</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.6215</c:v>
+                    <c:v>1.5005</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.9766</c:v>
+                    <c:v>0.8619</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1673,19 +1670,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4.2303</c:v>
+                  <c:v>2.0727</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.6066</c:v>
+                  <c:v>27.4432</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40.6602</c:v>
+                  <c:v>40.0787</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.6399</c:v>
+                  <c:v>46.1572</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51.0572</c:v>
+                  <c:v>49.4334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1734,19 +1731,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1048</c:v>
+                    <c:v>0.1509</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1522</c:v>
+                    <c:v>0.0285</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.504</c:v>
+                    <c:v>1.07</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.1698</c:v>
+                    <c:v>1.2127</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.8628</c:v>
+                    <c:v>1.776</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1758,19 +1755,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.3172</c:v>
+                    <c:v>0.1504</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2951</c:v>
+                    <c:v>0.1617</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.0156</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.199</c:v>
+                    <c:v>1.4094</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3564</c:v>
+                    <c:v>1.2126</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1820,19 +1817,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>-0.0544</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.094</c:v>
+                  <c:v>5.3325</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.5582</c:v>
+                  <c:v>29.5893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.8064</c:v>
+                  <c:v>42.3403</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47.4012</c:v>
+                  <c:v>48.335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,11 +1844,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2111288464"/>
-        <c:axId val="-2063463280"/>
+        <c:axId val="-2071476640"/>
+        <c:axId val="-2071470416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2111288464"/>
+        <c:axId val="-2071476640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,12 +1965,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2063463280"/>
+        <c:crossAx val="-2071470416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2063463280"/>
+        <c:axId val="-2071470416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,7 +2100,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2111288464"/>
+        <c:crossAx val="-2071476640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2325,19 +2322,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.2013</c:v>
+                    <c:v>0.415</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1507</c:v>
+                    <c:v>0.4628</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1746</c:v>
+                    <c:v>0.2436</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4543</c:v>
+                    <c:v>0.4768</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2055</c:v>
+                    <c:v>0.1564</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2349,19 +2346,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.5263</c:v>
+                    <c:v>0.6516</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0042</c:v>
+                    <c:v>0.0089</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.6984</c:v>
+                    <c:v>0.6216</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.0455</c:v>
+                    <c:v>0.124</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1793</c:v>
+                    <c:v>0.116</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2411,19 +2408,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>45.9148</c:v>
+                  <c:v>46.0564</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72.0127</c:v>
+                  <c:v>72.0174</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85.7411</c:v>
+                  <c:v>85.6617</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92.2821</c:v>
+                  <c:v>92.4318</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.1579</c:v>
+                  <c:v>96.0363</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2472,19 +2469,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.4507</c:v>
+                    <c:v>0.4659</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0662</c:v>
+                    <c:v>0.5245</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.1466</c:v>
+                    <c:v>0.2876</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.285</c:v>
+                    <c:v>0.4128</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1216</c:v>
+                    <c:v>0.1085</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2496,19 +2493,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.5396</c:v>
+                    <c:v>0.6168</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0004</c:v>
+                    <c:v>0.0016</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.6515</c:v>
+                    <c:v>0.4908</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.5284</c:v>
+                    <c:v>0.4107</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5422</c:v>
+                    <c:v>0.0847</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2558,19 +2555,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>47.3814</c:v>
+                  <c:v>47.3662</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.1272</c:v>
+                  <c:v>73.1284</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86.4124</c:v>
+                  <c:v>86.2517</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>92.85899999999999</c:v>
+                  <c:v>92.7977</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.2</c:v>
+                  <c:v>96.2599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2619,19 +2616,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.4349</c:v>
+                    <c:v>0.3557</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.8227</c:v>
+                    <c:v>1.585</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.4477</c:v>
+                    <c:v>0.8556</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.663</c:v>
+                    <c:v>0.8482</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5462</c:v>
+                    <c:v>0.1393</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2643,19 +2640,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>2.7731</c:v>
+                    <c:v>2.8429</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0013</c:v>
+                    <c:v>0.0026</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.674</c:v>
+                    <c:v>1.6628</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3.2911</c:v>
+                    <c:v>0.0771</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.1112</c:v>
+                    <c:v>0.2554</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2705,19 +2702,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>16.7898</c:v>
+                  <c:v>14.698</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.8323</c:v>
+                  <c:v>52.673</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>76.4547</c:v>
+                  <c:v>75.86279999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>87.8169</c:v>
+                  <c:v>87.2082</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>93.7071</c:v>
+                  <c:v>93.6232</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2766,19 +2763,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.091</c:v>
+                    <c:v>0.6962</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1799</c:v>
+                    <c:v>2.7549</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.6686</c:v>
+                    <c:v>0.6847</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.0448</c:v>
+                    <c:v>0.1429</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2491</c:v>
+                    <c:v>0.4181</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2790,19 +2787,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>2.1231</c:v>
+                    <c:v>1.2617</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1384</c:v>
+                    <c:v>0.2862</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.1161</c:v>
+                    <c:v>2.1148</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.1852</c:v>
+                    <c:v>0.7512</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3543</c:v>
+                    <c:v>0.0588</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2852,19 +2849,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.5315</c:v>
+                  <c:v>0.7128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.3952</c:v>
+                  <c:v>18.7906</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.952</c:v>
+                  <c:v>54.9852</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.9306</c:v>
+                  <c:v>77.1621</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88.7594</c:v>
+                  <c:v>88.2063</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2879,11 +2876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2041240448"/>
-        <c:axId val="-2041234224"/>
+        <c:axId val="-2071405968"/>
+        <c:axId val="-2071399744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2041240448"/>
+        <c:axId val="-2071405968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3000,12 +2997,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2041234224"/>
+        <c:crossAx val="-2071399744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2041234224"/>
+        <c:axId val="-2071399744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3135,7 +3132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2041240448"/>
+        <c:crossAx val="-2071405968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3357,19 +3354,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.2613</c:v>
+                    <c:v>1.7196</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.545</c:v>
+                    <c:v>1.1998</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.5085</c:v>
+                    <c:v>0.5437</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.2383</c:v>
+                    <c:v>1.0669</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5762</c:v>
+                    <c:v>0.0964</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3381,7 +3378,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.199</c:v>
+                    <c:v>0.2115</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>0.0012</c:v>
@@ -3390,10 +3387,10 @@
                     <c:v>1.207</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.4267</c:v>
+                    <c:v>0.4932</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.317</c:v>
+                    <c:v>0.4592</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3443,7 +3440,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>27.7955</c:v>
+                  <c:v>27.808</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>55.0174</c:v>
@@ -3452,10 +3449,10 @@
                   <c:v>74.116</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85.4407</c:v>
+                  <c:v>85.6217</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>92.38979999999999</c:v>
+                  <c:v>92.3493</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3504,19 +3501,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.7084</c:v>
+                    <c:v>1.7204</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.4371</c:v>
+                    <c:v>1.2043</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.55</c:v>
+                    <c:v>0.5115</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.7107</c:v>
+                    <c:v>0.8451</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.3422</c:v>
+                    <c:v>0.2693</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3528,19 +3525,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.1812</c:v>
+                    <c:v>0.8618</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.0027</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>1.1983</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.6423</c:v>
+                    <c:v>0.4537</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.3139</c:v>
+                    <c:v>0.324</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3590,19 +3587,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>27.2386</c:v>
+                  <c:v>27.2266</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.333</c:v>
+                  <c:v>54.3357</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>73.5843</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85.22</c:v>
+                  <c:v>85.1709</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>91.87479999999999</c:v>
+                  <c:v>92.0565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3651,19 +3648,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.326</c:v>
+                    <c:v>1.0693</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.6026</c:v>
+                    <c:v>3.0134</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.2885</c:v>
+                    <c:v>2.4151</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.6747</c:v>
+                    <c:v>1.869</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.9296</c:v>
+                    <c:v>0.4622</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3675,19 +3672,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>3.0192</c:v>
+                    <c:v>2.1967</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.0026</c:v>
+                    <c:v>0.0</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.8973</c:v>
+                    <c:v>2.877</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.993</c:v>
+                    <c:v>0.9728</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.2219</c:v>
+                    <c:v>0.4935</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3737,19 +3734,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>13.2379</c:v>
+                  <c:v>12.1899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.3341</c:v>
+                  <c:v>34.7688</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59.7872</c:v>
+                  <c:v>59.1898</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.9845</c:v>
+                  <c:v>76.5501</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>87.1712</c:v>
+                  <c:v>87.2419</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3798,19 +3795,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>0.091</c:v>
+                    <c:v>0.8273</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.1109</c:v>
+                    <c:v>2.8875</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.4406</c:v>
+                    <c:v>1.4329</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>1.3069</c:v>
+                    <c:v>0.7529</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0.5378</c:v>
+                    <c:v>1.1753</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3822,19 +3819,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>1.8051</c:v>
+                    <c:v>1.2616</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.2091</c:v>
+                    <c:v>0.3143</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.5837</c:v>
+                    <c:v>2.5431</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.6046</c:v>
+                    <c:v>0.6221</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.0418</c:v>
+                    <c:v>0.5344</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3884,19 +3881,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.5315</c:v>
+                  <c:v>0.7667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.3701</c:v>
+                  <c:v>14.2138</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.1048</c:v>
+                  <c:v>35.6079</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.846</c:v>
+                  <c:v>60.2594</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>78.706</c:v>
+                  <c:v>77.173</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3911,11 +3908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2041155888"/>
-        <c:axId val="-2041149664"/>
+        <c:axId val="-2085797280"/>
+        <c:axId val="-2085791056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2041155888"/>
+        <c:axId val="-2085797280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4032,12 +4029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2041149664"/>
+        <c:crossAx val="-2085791056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2041149664"/>
+        <c:axId val="-2085791056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4167,7 +4164,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2041155888"/>
+        <c:crossAx val="-2085797280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6609,915 +6606,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="out"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="D4">
-            <v>2</v>
-          </cell>
-          <cell r="E4">
-            <v>0</v>
-          </cell>
-          <cell r="F4">
-            <v>0.1643</v>
-          </cell>
-          <cell r="G4">
-            <v>2.8054999999999999</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>4</v>
-          </cell>
-          <cell r="E5">
-            <v>0</v>
-          </cell>
-          <cell r="F5">
-            <v>5.0853000000000002</v>
-          </cell>
-          <cell r="G5">
-            <v>1.5634999999999999</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>8</v>
-          </cell>
-          <cell r="E6">
-            <v>0</v>
-          </cell>
-          <cell r="F6">
-            <v>3.8491</v>
-          </cell>
-          <cell r="G6">
-            <v>4.5976999999999997</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>16</v>
-          </cell>
-          <cell r="E7">
-            <v>0.99880000000000002</v>
-          </cell>
-          <cell r="F7">
-            <v>1.1251</v>
-          </cell>
-          <cell r="G7">
-            <v>1.5762</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>32</v>
-          </cell>
-          <cell r="E8">
-            <v>-1.0606</v>
-          </cell>
-          <cell r="F8">
-            <v>14.9473</v>
-          </cell>
-          <cell r="G8">
-            <v>0.85389999999999999</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>-1.5775999999999999</v>
-          </cell>
-          <cell r="F10">
-            <v>6.0461</v>
-          </cell>
-          <cell r="G10">
-            <v>7.6142000000000003</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>0</v>
-          </cell>
-          <cell r="F11">
-            <v>6.3746999999999998</v>
-          </cell>
-          <cell r="G11">
-            <v>4.8391999999999999</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>0.47599999999999998</v>
-          </cell>
-          <cell r="F12">
-            <v>24.1937</v>
-          </cell>
-          <cell r="G12">
-            <v>4.7892999999999999</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>2.4679000000000002</v>
-          </cell>
-          <cell r="F13">
-            <v>7.1369999999999996</v>
-          </cell>
-          <cell r="G13">
-            <v>3.3473999999999999</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>3.3096000000000001</v>
-          </cell>
-          <cell r="F14">
-            <v>4.7234999999999996</v>
-          </cell>
-          <cell r="G14">
-            <v>16.872199999999999</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>0</v>
-          </cell>
-          <cell r="F16">
-            <v>3.7170000000000001</v>
-          </cell>
-          <cell r="G16">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>-1.3613</v>
-          </cell>
-          <cell r="F17">
-            <v>8.2149999999999999</v>
-          </cell>
-          <cell r="G17">
-            <v>4.9702999999999999</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>0.4249</v>
-          </cell>
-          <cell r="F18">
-            <v>0.4249</v>
-          </cell>
-          <cell r="G18">
-            <v>12.2194</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>12.230700000000001</v>
-          </cell>
-          <cell r="F19">
-            <v>61.433300000000003</v>
-          </cell>
-          <cell r="G19">
-            <v>24.942699999999999</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>-3.1762000000000001</v>
-          </cell>
-          <cell r="F20">
-            <v>42.6265</v>
-          </cell>
-          <cell r="G20">
-            <v>23.130800000000001</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="E22">
-            <v>0</v>
-          </cell>
-          <cell r="F22">
-            <v>1.9496</v>
-          </cell>
-          <cell r="G22">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="E23">
-            <v>0</v>
-          </cell>
-          <cell r="F23">
-            <v>1.6688000000000001</v>
-          </cell>
-          <cell r="G23">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="E24">
-            <v>0.45829999999999999</v>
-          </cell>
-          <cell r="F24">
-            <v>3.8898999999999999</v>
-          </cell>
-          <cell r="G24">
-            <v>3.032</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="E25">
-            <v>-1.6879</v>
-          </cell>
-          <cell r="F25">
-            <v>63.305999999999997</v>
-          </cell>
-          <cell r="G25">
-            <v>50.4649</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="E26">
-            <v>-1.8727</v>
-          </cell>
-          <cell r="F26">
-            <v>11.662000000000001</v>
-          </cell>
-          <cell r="G26">
-            <v>23.3337</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="E29">
-            <v>13.2614</v>
-          </cell>
-          <cell r="F29">
-            <v>1.8876999999999999</v>
-          </cell>
-          <cell r="G29">
-            <v>0.21709999999999999</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="E30">
-            <v>9.6968999999999994</v>
-          </cell>
-          <cell r="F30">
-            <v>9.8062000000000005</v>
-          </cell>
-          <cell r="G30">
-            <v>3.1705000000000001</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="E31">
-            <v>11.649900000000001</v>
-          </cell>
-          <cell r="F31">
-            <v>3.7254</v>
-          </cell>
-          <cell r="G31">
-            <v>6.0811999999999999</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="E32">
-            <v>12.2293</v>
-          </cell>
-          <cell r="F32">
-            <v>0.94810000000000005</v>
-          </cell>
-          <cell r="G32">
-            <v>4.6520000000000001</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="E33">
-            <v>12.5162</v>
-          </cell>
-          <cell r="F33">
-            <v>2.7187000000000001</v>
-          </cell>
-          <cell r="G33">
-            <v>1.0156000000000001</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="E35">
-            <v>5.6441999999999997</v>
-          </cell>
-          <cell r="F35">
-            <v>5.6441999999999997</v>
-          </cell>
-          <cell r="G35">
-            <v>1.5902000000000001</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="E36">
-            <v>12.847300000000001</v>
-          </cell>
-          <cell r="F36">
-            <v>12.8005</v>
-          </cell>
-          <cell r="G36">
-            <v>0.54349999999999998</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="E37">
-            <v>10.454700000000001</v>
-          </cell>
-          <cell r="F37">
-            <v>15.8614</v>
-          </cell>
-          <cell r="G37">
-            <v>0.79569999999999996</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="E38">
-            <v>16.051400000000001</v>
-          </cell>
-          <cell r="F38">
-            <v>22.700700000000001</v>
-          </cell>
-          <cell r="G38">
-            <v>3.2416999999999998</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="E39">
-            <v>15.5762</v>
-          </cell>
-          <cell r="F39">
-            <v>1.0969</v>
-          </cell>
-          <cell r="G39">
-            <v>18.361599999999999</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="E41">
-            <v>0</v>
-          </cell>
-          <cell r="F41">
-            <v>0</v>
-          </cell>
-          <cell r="G41">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="E42">
-            <v>0</v>
-          </cell>
-          <cell r="F42">
-            <v>0</v>
-          </cell>
-          <cell r="G42">
-            <v>6.8838999999999997</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="E43">
-            <v>10.8827</v>
-          </cell>
-          <cell r="F43">
-            <v>4.3000999999999996</v>
-          </cell>
-          <cell r="G43">
-            <v>1.9446000000000001</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="E44">
-            <v>15.3573</v>
-          </cell>
-          <cell r="F44">
-            <v>19.654399999999999</v>
-          </cell>
-          <cell r="G44">
-            <v>26.616199999999999</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="E45">
-            <v>16.158799999999999</v>
-          </cell>
-          <cell r="F45">
-            <v>27.836600000000001</v>
-          </cell>
-          <cell r="G45">
-            <v>18.257000000000001</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="E47">
-            <v>0</v>
-          </cell>
-          <cell r="F47">
-            <v>0</v>
-          </cell>
-          <cell r="G47">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="E48">
-            <v>0</v>
-          </cell>
-          <cell r="F48">
-            <v>0</v>
-          </cell>
-          <cell r="G48">
-            <v>1.7171000000000001</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="E49">
-            <v>1.5734999999999999</v>
-          </cell>
-          <cell r="F49">
-            <v>1.5734999999999999</v>
-          </cell>
-          <cell r="G49">
-            <v>3.6619999999999999</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="E50">
-            <v>10.470499999999999</v>
-          </cell>
-          <cell r="F50">
-            <v>7.9917999999999996</v>
-          </cell>
-          <cell r="G50">
-            <v>44.195099999999996</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="E51">
-            <v>9.7014999999999993</v>
-          </cell>
-          <cell r="F51">
-            <v>1.7801</v>
-          </cell>
-          <cell r="G51">
-            <v>32.2425</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="E54">
-            <v>13.2614</v>
-          </cell>
-          <cell r="F54">
-            <v>1.8876999999999999</v>
-          </cell>
-          <cell r="G54">
-            <v>0.21709999999999999</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="E55">
-            <v>11.326700000000001</v>
-          </cell>
-          <cell r="F55">
-            <v>11.436</v>
-          </cell>
-          <cell r="G55">
-            <v>1.923</v>
-          </cell>
-        </row>
-        <row r="56">
-          <cell r="E56">
-            <v>40</v>
-          </cell>
-          <cell r="F56">
-            <v>9.5740999999999996</v>
-          </cell>
-          <cell r="G56">
-            <v>1.5264</v>
-          </cell>
-        </row>
-        <row r="57">
-          <cell r="E57">
-            <v>60.003700000000002</v>
-          </cell>
-          <cell r="F57">
-            <v>0.55549999999999999</v>
-          </cell>
-          <cell r="G57">
-            <v>1.8740000000000001</v>
-          </cell>
-        </row>
-        <row r="58">
-          <cell r="E58">
-            <v>77.846299999999999</v>
-          </cell>
-          <cell r="F58">
-            <v>4.8650000000000002</v>
-          </cell>
-          <cell r="G58">
-            <v>0.23069999999999999</v>
-          </cell>
-        </row>
-        <row r="60">
-          <cell r="E60">
-            <v>5.6441999999999997</v>
-          </cell>
-          <cell r="F60">
-            <v>5.6441999999999997</v>
-          </cell>
-          <cell r="G60">
-            <v>1.5902000000000001</v>
-          </cell>
-        </row>
-        <row r="61">
-          <cell r="E61">
-            <v>12.847300000000001</v>
-          </cell>
-          <cell r="F61">
-            <v>12.8005</v>
-          </cell>
-          <cell r="G61">
-            <v>0.54349999999999998</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="E62">
-            <v>10.454700000000001</v>
-          </cell>
-          <cell r="F62">
-            <v>15.8614</v>
-          </cell>
-          <cell r="G62">
-            <v>0.79569999999999996</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="E63">
-            <v>38.173999999999999</v>
-          </cell>
-          <cell r="F63">
-            <v>5.0109000000000004</v>
-          </cell>
-          <cell r="G63">
-            <v>6.3003</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="E64">
-            <v>61.310600000000001</v>
-          </cell>
-          <cell r="F64">
-            <v>14.902100000000001</v>
-          </cell>
-          <cell r="G64">
-            <v>8.1167999999999996</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="E66">
-            <v>0</v>
-          </cell>
-          <cell r="F66">
-            <v>0</v>
-          </cell>
-          <cell r="G66">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="E67">
-            <v>0</v>
-          </cell>
-          <cell r="F67">
-            <v>0</v>
-          </cell>
-          <cell r="G67">
-            <v>6.8838999999999997</v>
-          </cell>
-        </row>
-        <row r="68">
-          <cell r="E68">
-            <v>10.8827</v>
-          </cell>
-          <cell r="F68">
-            <v>4.3000999999999996</v>
-          </cell>
-          <cell r="G68">
-            <v>1.9446000000000001</v>
-          </cell>
-        </row>
-        <row r="69">
-          <cell r="E69">
-            <v>26.523900000000001</v>
-          </cell>
-          <cell r="F69">
-            <v>23.739000000000001</v>
-          </cell>
-          <cell r="G69">
-            <v>16.110499999999998</v>
-          </cell>
-        </row>
-        <row r="70">
-          <cell r="E70">
-            <v>24.443300000000001</v>
-          </cell>
-          <cell r="F70">
-            <v>33.001899999999999</v>
-          </cell>
-          <cell r="G70">
-            <v>16.8432</v>
-          </cell>
-        </row>
-        <row r="72">
-          <cell r="E72">
-            <v>0</v>
-          </cell>
-          <cell r="F72">
-            <v>0</v>
-          </cell>
-          <cell r="G72">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="73">
-          <cell r="E73">
-            <v>0</v>
-          </cell>
-          <cell r="F73">
-            <v>0</v>
-          </cell>
-          <cell r="G73">
-            <v>1.7171000000000001</v>
-          </cell>
-        </row>
-        <row r="74">
-          <cell r="E74">
-            <v>1.5734999999999999</v>
-          </cell>
-          <cell r="F74">
-            <v>1.5734999999999999</v>
-          </cell>
-          <cell r="G74">
-            <v>3.6619999999999999</v>
-          </cell>
-        </row>
-        <row r="75">
-          <cell r="E75">
-            <v>8.6221999999999994</v>
-          </cell>
-          <cell r="F75">
-            <v>2.4939</v>
-          </cell>
-          <cell r="G75">
-            <v>49.9315</v>
-          </cell>
-        </row>
-        <row r="76">
-          <cell r="E76">
-            <v>14.291700000000001</v>
-          </cell>
-          <cell r="F76">
-            <v>6.7023000000000001</v>
-          </cell>
-          <cell r="G76">
-            <v>24.596</v>
-          </cell>
-        </row>
-        <row r="79">
-          <cell r="E79">
-            <v>0</v>
-          </cell>
-          <cell r="F79">
-            <v>0</v>
-          </cell>
-          <cell r="G79">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="80">
-          <cell r="E80">
-            <v>0</v>
-          </cell>
-          <cell r="F80">
-            <v>0</v>
-          </cell>
-          <cell r="G80">
-            <v>3.9342999999999999</v>
-          </cell>
-        </row>
-        <row r="81">
-          <cell r="E81">
-            <v>27.0684</v>
-          </cell>
-          <cell r="F81">
-            <v>4.4432</v>
-          </cell>
-          <cell r="G81">
-            <v>5.7645999999999997</v>
-          </cell>
-        </row>
-        <row r="82">
-          <cell r="E82">
-            <v>54.4985</v>
-          </cell>
-          <cell r="F82">
-            <v>1.7824</v>
-          </cell>
-          <cell r="G82">
-            <v>1.4715</v>
-          </cell>
-        </row>
-        <row r="83">
-          <cell r="E83">
-            <v>74.558700000000002</v>
-          </cell>
-          <cell r="F83">
-            <v>5.8056999999999999</v>
-          </cell>
-          <cell r="G83">
-            <v>0.88129999999999997</v>
-          </cell>
-        </row>
-        <row r="85">
-          <cell r="E85">
-            <v>0</v>
-          </cell>
-          <cell r="F85">
-            <v>0</v>
-          </cell>
-          <cell r="G85">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="86">
-          <cell r="E86">
-            <v>0</v>
-          </cell>
-          <cell r="F86">
-            <v>0</v>
-          </cell>
-          <cell r="G86">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="87">
-          <cell r="E87">
-            <v>0</v>
-          </cell>
-          <cell r="F87">
-            <v>0</v>
-          </cell>
-          <cell r="G87">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="88">
-          <cell r="E88">
-            <v>31.691500000000001</v>
-          </cell>
-          <cell r="F88">
-            <v>8.5687999999999995</v>
-          </cell>
-          <cell r="G88">
-            <v>9.1980000000000004</v>
-          </cell>
-        </row>
-        <row r="89">
-          <cell r="E89">
-            <v>53.721400000000003</v>
-          </cell>
-          <cell r="F89">
-            <v>16.9374</v>
-          </cell>
-          <cell r="G89">
-            <v>1.2712000000000001</v>
-          </cell>
-        </row>
-        <row r="91">
-          <cell r="E91">
-            <v>0</v>
-          </cell>
-          <cell r="F91">
-            <v>0</v>
-          </cell>
-          <cell r="G91">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="92">
-          <cell r="E92">
-            <v>0</v>
-          </cell>
-          <cell r="F92">
-            <v>0</v>
-          </cell>
-          <cell r="G92">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="93">
-          <cell r="E93">
-            <v>0</v>
-          </cell>
-          <cell r="F93">
-            <v>0</v>
-          </cell>
-          <cell r="G93">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="94">
-          <cell r="E94">
-            <v>8.9197000000000006</v>
-          </cell>
-          <cell r="F94">
-            <v>18.812200000000001</v>
-          </cell>
-          <cell r="G94">
-            <v>21.910599999999999</v>
-          </cell>
-        </row>
-        <row r="95">
-          <cell r="E95">
-            <v>10.476100000000001</v>
-          </cell>
-          <cell r="F95">
-            <v>42.1678</v>
-          </cell>
-          <cell r="G95">
-            <v>22.694900000000001</v>
-          </cell>
-        </row>
-        <row r="97">
-          <cell r="E97">
-            <v>0</v>
-          </cell>
-          <cell r="F97">
-            <v>0</v>
-          </cell>
-          <cell r="G97">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="98">
-          <cell r="E98">
-            <v>0</v>
-          </cell>
-          <cell r="F98">
-            <v>0</v>
-          </cell>
-          <cell r="G98">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="99">
-          <cell r="E99">
-            <v>0</v>
-          </cell>
-          <cell r="F99">
-            <v>0</v>
-          </cell>
-          <cell r="G99">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="100">
-          <cell r="E100">
-            <v>0.31190000000000001</v>
-          </cell>
-          <cell r="F100">
-            <v>6.4145000000000003</v>
-          </cell>
-          <cell r="G100">
-            <v>8.2644000000000002</v>
-          </cell>
-        </row>
-        <row r="101">
-          <cell r="E101">
-            <v>0.1547</v>
-          </cell>
-          <cell r="F101">
-            <v>7.9634999999999998</v>
-          </cell>
-          <cell r="G101">
-            <v>24.325700000000001</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7786,7 +6874,7 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7853,10 +6941,10 @@
         <v>19.162099999999999</v>
       </c>
       <c r="F4">
-        <v>0.93079999999999996</v>
+        <v>0.80279999999999996</v>
       </c>
       <c r="G4">
-        <v>0.80169999999999997</v>
+        <v>1.2476</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -7873,13 +6961,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>31.6127</v>
+        <v>31.4453</v>
       </c>
       <c r="F5">
-        <v>0.39550000000000002</v>
+        <v>1.1751</v>
       </c>
       <c r="G5">
-        <v>0.56310000000000004</v>
+        <v>0.90110000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7896,13 +6984,13 @@
         <v>8</v>
       </c>
       <c r="E6">
-        <v>36.839599999999997</v>
+        <v>37.327800000000003</v>
       </c>
       <c r="F6">
-        <v>0.5383</v>
+        <v>1.4831000000000001</v>
       </c>
       <c r="G6">
-        <v>0.91</v>
+        <v>0.71330000000000005</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7919,13 +7007,13 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>40.140799999999999</v>
+        <v>40.445700000000002</v>
       </c>
       <c r="F7">
-        <v>1.0137</v>
+        <v>0.93130000000000002</v>
       </c>
       <c r="G7">
-        <v>1.0961000000000001</v>
+        <v>0.32679999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7942,13 +7030,13 @@
         <v>32</v>
       </c>
       <c r="E8">
-        <v>41.924300000000002</v>
+        <v>42.104500000000002</v>
       </c>
       <c r="F8">
-        <v>0.32490000000000002</v>
+        <v>0.69350000000000001</v>
       </c>
       <c r="G8">
-        <v>0.29120000000000001</v>
+        <v>0.34210000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7965,13 +7053,13 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>19.715399999999999</v>
+        <v>19.697500000000002</v>
       </c>
       <c r="F10">
-        <v>0.16789999999999999</v>
+        <v>0.15260000000000001</v>
       </c>
       <c r="G10">
-        <v>1.5408999999999999</v>
+        <v>1.5588</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -7991,10 +7079,10 @@
         <v>31.972799999999999</v>
       </c>
       <c r="F11">
-        <v>2.0999999999999999E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="G11">
-        <v>0.48959999999999998</v>
+        <v>1.1747000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -8011,13 +7099,13 @@
         <v>8</v>
       </c>
       <c r="E12">
-        <v>38.417400000000001</v>
+        <v>38.503599999999999</v>
       </c>
       <c r="F12">
-        <v>1.0931999999999999</v>
+        <v>1.3906000000000001</v>
       </c>
       <c r="G12">
-        <v>0.19170000000000001</v>
+        <v>0.1055</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -8034,13 +7122,13 @@
         <v>16</v>
       </c>
       <c r="E13">
-        <v>41.256300000000003</v>
+        <v>41.464700000000001</v>
       </c>
       <c r="F13">
-        <v>0.67820000000000003</v>
+        <v>0.7429</v>
       </c>
       <c r="G13">
-        <v>0.62680000000000002</v>
+        <v>1.1519999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -8057,13 +7145,13 @@
         <v>32</v>
       </c>
       <c r="E14">
-        <v>42.879399999999997</v>
+        <v>43.221499999999999</v>
       </c>
       <c r="F14">
-        <v>0.77690000000000003</v>
+        <v>0.2732</v>
       </c>
       <c r="G14">
-        <v>0.99009999999999998</v>
+        <v>0.50390000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -8080,13 +7168,13 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>12.691000000000001</v>
+        <v>11.890599999999999</v>
       </c>
       <c r="F16">
-        <v>2.8994</v>
+        <v>2.1093000000000002</v>
       </c>
       <c r="G16">
-        <v>0.29330000000000001</v>
+        <v>1.0842000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -8106,10 +7194,10 @@
         <v>25.229199999999999</v>
       </c>
       <c r="F17">
-        <v>2.0999999999999999E-3</v>
+        <v>7.6E-3</v>
       </c>
       <c r="G17">
-        <v>1.3297000000000001</v>
+        <v>2.548</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -8132,7 +7220,7 @@
         <v>1.9423999999999999</v>
       </c>
       <c r="G18">
-        <v>1.2372000000000001</v>
+        <v>2.3475999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -8149,13 +7237,13 @@
         <v>16</v>
       </c>
       <c r="E19">
-        <v>40.873800000000003</v>
+        <v>40.423299999999998</v>
       </c>
       <c r="F19">
-        <v>1.8247</v>
+        <v>1.3339000000000001</v>
       </c>
       <c r="G19">
-        <v>0.2039</v>
+        <v>1.8070999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -8172,13 +7260,13 @@
         <v>32</v>
       </c>
       <c r="E20">
-        <v>44.361600000000003</v>
+        <v>43.3887</v>
       </c>
       <c r="F20">
-        <v>1.2505999999999999</v>
+        <v>2.4016000000000002</v>
       </c>
       <c r="G20">
-        <v>0.14149999999999999</v>
+        <v>1.0542</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -8195,13 +7283,13 @@
         <v>2</v>
       </c>
       <c r="E22">
-        <v>0.59060000000000001</v>
+        <v>0.83860000000000001</v>
       </c>
       <c r="F22">
-        <v>1.1821999999999999</v>
+        <v>1.032</v>
       </c>
       <c r="G22">
-        <v>0.94179999999999997</v>
+        <v>0.434</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -8218,13 +7306,13 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>13.4313</v>
+        <v>13.450699999999999</v>
       </c>
       <c r="F23">
-        <v>0.15040000000000001</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="G23">
-        <v>6.0999999999999999E-2</v>
+        <v>2.7385999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -8244,7 +7332,7 @@
         <v>24.892499999999998</v>
       </c>
       <c r="F24">
-        <v>1.5911999999999999</v>
+        <v>1.6113</v>
       </c>
       <c r="G24">
         <v>1.1856</v>
@@ -8264,13 +7352,13 @@
         <v>16</v>
       </c>
       <c r="E25">
-        <v>34.918399999999998</v>
+        <v>35.279600000000002</v>
       </c>
       <c r="F25">
-        <v>0.92420000000000002</v>
+        <v>2.5150000000000001</v>
       </c>
       <c r="G25">
-        <v>1.4012</v>
+        <v>0.52490000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -8287,13 +7375,13 @@
         <v>32</v>
       </c>
       <c r="E26">
-        <v>40.2117</v>
+        <v>40.7455</v>
       </c>
       <c r="F26">
-        <v>0.2077</v>
+        <v>1.0472999999999999</v>
       </c>
       <c r="G26">
-        <v>0.95840000000000003</v>
+        <v>0.64419999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -8318,13 +7406,13 @@
         <v>2</v>
       </c>
       <c r="E29">
-        <v>25.0944</v>
+        <v>25.102799999999998</v>
       </c>
       <c r="F29">
-        <v>1.048</v>
+        <v>1.0596000000000001</v>
       </c>
       <c r="G29">
-        <v>8.3999999999999995E-3</v>
+        <v>0.57640000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -8341,13 +7429,13 @@
         <v>4</v>
       </c>
       <c r="E30">
-        <v>37.7742</v>
+        <v>37.781999999999996</v>
       </c>
       <c r="F30">
-        <v>0.41620000000000001</v>
+        <v>0.82950000000000002</v>
       </c>
       <c r="G30">
-        <v>1.83E-2</v>
+        <v>0.41010000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -8364,13 +7452,13 @@
         <v>8</v>
       </c>
       <c r="E31">
-        <v>44.496499999999997</v>
+        <v>44.383000000000003</v>
       </c>
       <c r="F31">
-        <v>0.90839999999999999</v>
+        <v>0.67379999999999995</v>
       </c>
       <c r="G31">
-        <v>0.41599999999999998</v>
+        <v>1.0938000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -8387,13 +7475,13 @@
         <v>16</v>
       </c>
       <c r="E32">
-        <v>46.989800000000002</v>
+        <v>47.439100000000003</v>
       </c>
       <c r="F32">
-        <v>0.28370000000000001</v>
+        <v>1.3469</v>
       </c>
       <c r="G32">
-        <v>3.1206</v>
+        <v>1.6700999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -8410,13 +7498,13 @@
         <v>32</v>
       </c>
       <c r="E33">
-        <v>48.837400000000002</v>
+        <v>49.066699999999997</v>
       </c>
       <c r="F33">
-        <v>0.53739999999999999</v>
+        <v>0.92059999999999997</v>
       </c>
       <c r="G33">
-        <v>0.67649999999999999</v>
+        <v>0.81389999999999996</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -8433,13 +7521,13 @@
         <v>2</v>
       </c>
       <c r="E35">
-        <v>27.674399999999999</v>
+        <v>27.683299999999999</v>
       </c>
       <c r="F35">
-        <v>1.0955999999999999</v>
+        <v>1.1045</v>
       </c>
       <c r="G35">
-        <v>1.12E-2</v>
+        <v>2.3E-3</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -8459,10 +7547,10 @@
         <v>41.154000000000003</v>
       </c>
       <c r="F36">
-        <v>0.42149999999999999</v>
+        <v>0.83620000000000005</v>
       </c>
       <c r="G36">
-        <v>8.9999999999999998E-4</v>
+        <v>0.42459999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -8485,7 +7573,7 @@
         <v>0.79559999999999997</v>
       </c>
       <c r="G37">
-        <v>0.52600000000000002</v>
+        <v>1.1013999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -8502,13 +7590,13 @@
         <v>16</v>
       </c>
       <c r="E38">
-        <v>51.383299999999998</v>
+        <v>51.081200000000003</v>
       </c>
       <c r="F38">
-        <v>1.1124000000000001</v>
+        <v>0.89529999999999998</v>
       </c>
       <c r="G38">
-        <v>0.45100000000000001</v>
+        <v>0.98919999999999997</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -8525,13 +7613,13 @@
         <v>32</v>
       </c>
       <c r="E39">
-        <v>53.158799999999999</v>
+        <v>52.924300000000002</v>
       </c>
       <c r="F39">
-        <v>0.4209</v>
+        <v>0.90620000000000001</v>
       </c>
       <c r="G39">
-        <v>0.83850000000000002</v>
+        <v>0.91410000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -8548,13 +7636,13 @@
         <v>2</v>
       </c>
       <c r="E41">
-        <v>4.2302999999999997</v>
+        <v>2.0727000000000002</v>
       </c>
       <c r="F41">
-        <v>0.13639999999999999</v>
+        <v>7.5700000000000003E-2</v>
       </c>
       <c r="G41">
-        <v>4.8999999999999998E-3</v>
+        <v>1.1493</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -8571,13 +7659,13 @@
         <v>4</v>
       </c>
       <c r="E42">
-        <v>28.6066</v>
+        <v>27.443200000000001</v>
       </c>
       <c r="F42">
-        <v>0.51049999999999995</v>
+        <v>0.96240000000000003</v>
       </c>
       <c r="G42">
-        <v>2E-3</v>
+        <v>0.50009999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -8594,13 +7682,13 @@
         <v>8</v>
       </c>
       <c r="E43">
-        <v>40.660200000000003</v>
+        <v>40.078699999999998</v>
       </c>
       <c r="F43">
-        <v>1.4E-3</v>
+        <v>0.7157</v>
       </c>
       <c r="G43">
-        <v>1.2230000000000001</v>
+        <v>1.6391</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -8617,13 +7705,13 @@
         <v>16</v>
       </c>
       <c r="E44">
-        <v>46.639899999999997</v>
+        <v>46.157200000000003</v>
       </c>
       <c r="F44">
-        <v>0.62150000000000005</v>
+        <v>1.5004999999999999</v>
       </c>
       <c r="G44">
-        <v>0.50790000000000002</v>
+        <v>4.8859000000000004</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -8640,13 +7728,13 @@
         <v>32</v>
       </c>
       <c r="E45">
-        <v>51.057200000000002</v>
+        <v>49.433399999999999</v>
       </c>
       <c r="F45">
-        <v>0.97660000000000002</v>
+        <v>0.8619</v>
       </c>
       <c r="G45">
-        <v>0.72399999999999998</v>
+        <v>1.7432000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -8663,13 +7751,13 @@
         <v>2</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>-5.4399999999999997E-2</v>
       </c>
       <c r="F47">
-        <v>0.31719999999999998</v>
+        <v>0.15040000000000001</v>
       </c>
       <c r="G47">
-        <v>0.1048</v>
+        <v>0.15090000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -8686,13 +7774,13 @@
         <v>4</v>
       </c>
       <c r="E48">
-        <v>7.0940000000000003</v>
+        <v>5.3324999999999996</v>
       </c>
       <c r="F48">
-        <v>0.29509999999999997</v>
+        <v>0.16170000000000001</v>
       </c>
       <c r="G48">
-        <v>0.1522</v>
+        <v>2.8500000000000001E-2</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -8709,13 +7797,13 @@
         <v>8</v>
       </c>
       <c r="E49">
-        <v>30.558199999999999</v>
+        <v>29.589300000000001</v>
       </c>
       <c r="F49">
-        <v>1.5599999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>0.504</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -8732,13 +7820,13 @@
         <v>16</v>
       </c>
       <c r="E50">
-        <v>41.806399999999996</v>
+        <v>42.340299999999999</v>
       </c>
       <c r="F50">
-        <v>1.1990000000000001</v>
+        <v>1.4094</v>
       </c>
       <c r="G50">
-        <v>0.16980000000000001</v>
+        <v>1.2126999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -8755,13 +7843,13 @@
         <v>32</v>
       </c>
       <c r="E51">
-        <v>47.401200000000003</v>
+        <v>48.335000000000001</v>
       </c>
       <c r="F51">
-        <v>0.35639999999999999</v>
+        <v>1.2125999999999999</v>
       </c>
       <c r="G51">
-        <v>0.86280000000000001</v>
+        <v>1.776</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -8786,13 +7874,13 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <v>45.9148</v>
+        <v>46.056399999999996</v>
       </c>
       <c r="F54">
-        <v>0.52629999999999999</v>
+        <v>0.65159999999999996</v>
       </c>
       <c r="G54">
-        <v>0.20130000000000001</v>
+        <v>0.41499999999999998</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -8809,13 +7897,13 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>72.012699999999995</v>
+        <v>72.017399999999995</v>
       </c>
       <c r="F55">
-        <v>4.1999999999999997E-3</v>
+        <v>8.8999999999999999E-3</v>
       </c>
       <c r="G55">
-        <v>0.1507</v>
+        <v>0.46279999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -8832,13 +7920,13 @@
         <v>8</v>
       </c>
       <c r="E56">
-        <v>85.741100000000003</v>
+        <v>85.661699999999996</v>
       </c>
       <c r="F56">
-        <v>0.69840000000000002</v>
+        <v>0.62160000000000004</v>
       </c>
       <c r="G56">
-        <v>0.17460000000000001</v>
+        <v>0.24360000000000001</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -8855,13 +7943,13 @@
         <v>16</v>
       </c>
       <c r="E57">
-        <v>92.2821</v>
+        <v>92.431799999999996</v>
       </c>
       <c r="F57">
-        <v>4.5499999999999999E-2</v>
+        <v>0.124</v>
       </c>
       <c r="G57">
-        <v>0.45429999999999998</v>
+        <v>0.4768</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -8878,13 +7966,13 @@
         <v>32</v>
       </c>
       <c r="E58">
-        <v>96.157899999999998</v>
+        <v>96.036299999999997</v>
       </c>
       <c r="F58">
-        <v>0.17929999999999999</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="G58">
-        <v>0.20549999999999999</v>
+        <v>0.15640000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -8901,13 +7989,13 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>47.381399999999999</v>
+        <v>47.366199999999999</v>
       </c>
       <c r="F60">
-        <v>0.53959999999999997</v>
+        <v>0.61680000000000001</v>
       </c>
       <c r="G60">
-        <v>0.45069999999999999</v>
+        <v>0.46589999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -8924,13 +8012,13 @@
         <v>4</v>
       </c>
       <c r="E61">
-        <v>73.127200000000002</v>
+        <v>73.128399999999999</v>
       </c>
       <c r="F61">
-        <v>4.0000000000000002E-4</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="G61">
-        <v>6.6199999999999995E-2</v>
+        <v>0.52449999999999997</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -8947,13 +8035,13 @@
         <v>8</v>
       </c>
       <c r="E62">
-        <v>86.412400000000005</v>
+        <v>86.2517</v>
       </c>
       <c r="F62">
-        <v>0.65149999999999997</v>
+        <v>0.49080000000000001</v>
       </c>
       <c r="G62">
-        <v>0.14660000000000001</v>
+        <v>0.28760000000000002</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -8970,13 +8058,13 @@
         <v>16</v>
       </c>
       <c r="E63">
-        <v>92.858999999999995</v>
+        <v>92.797700000000006</v>
       </c>
       <c r="F63">
-        <v>0.52839999999999998</v>
+        <v>0.41070000000000001</v>
       </c>
       <c r="G63">
-        <v>0.28499999999999998</v>
+        <v>0.4128</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -8993,13 +8081,13 @@
         <v>32</v>
       </c>
       <c r="E64">
-        <v>96.2</v>
+        <v>96.259900000000002</v>
       </c>
       <c r="F64">
-        <v>0.54220000000000002</v>
+        <v>8.4699999999999998E-2</v>
       </c>
       <c r="G64">
-        <v>0.1216</v>
+        <v>0.1085</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -9016,13 +8104,13 @@
         <v>2</v>
       </c>
       <c r="E66">
-        <v>16.7898</v>
+        <v>14.698</v>
       </c>
       <c r="F66">
-        <v>2.7730999999999999</v>
+        <v>2.8429000000000002</v>
       </c>
       <c r="G66">
-        <v>0.43490000000000001</v>
+        <v>0.35570000000000002</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -9039,13 +8127,13 @@
         <v>4</v>
       </c>
       <c r="E67">
-        <v>53.832299999999996</v>
+        <v>52.673000000000002</v>
       </c>
       <c r="F67">
-        <v>1.2999999999999999E-3</v>
+        <v>2.5999999999999999E-3</v>
       </c>
       <c r="G67">
-        <v>0.82269999999999999</v>
+        <v>1.585</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -9062,13 +8150,13 @@
         <v>8</v>
       </c>
       <c r="E68">
-        <v>76.454700000000003</v>
+        <v>75.862799999999993</v>
       </c>
       <c r="F68">
-        <v>1.6739999999999999</v>
+        <v>1.6628000000000001</v>
       </c>
       <c r="G68">
-        <v>0.44769999999999999</v>
+        <v>0.85560000000000003</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -9085,13 +8173,13 @@
         <v>16</v>
       </c>
       <c r="E69">
-        <v>87.816900000000004</v>
+        <v>87.208200000000005</v>
       </c>
       <c r="F69">
-        <v>3.2911000000000001</v>
+        <v>7.7100000000000002E-2</v>
       </c>
       <c r="G69">
-        <v>0.66300000000000003</v>
+        <v>0.84819999999999995</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -9108,13 +8196,13 @@
         <v>32</v>
       </c>
       <c r="E70">
-        <v>93.707099999999997</v>
+        <v>93.623199999999997</v>
       </c>
       <c r="F70">
-        <v>0.11119999999999999</v>
+        <v>0.25540000000000002</v>
       </c>
       <c r="G70">
-        <v>0.54620000000000002</v>
+        <v>0.13930000000000001</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -9131,13 +8219,13 @@
         <v>2</v>
       </c>
       <c r="E72">
-        <v>1.5315000000000001</v>
+        <v>0.71279999999999999</v>
       </c>
       <c r="F72">
-        <v>2.1231</v>
+        <v>1.2617</v>
       </c>
       <c r="G72">
-        <v>9.0999999999999998E-2</v>
+        <v>0.69620000000000004</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -9154,13 +8242,13 @@
         <v>4</v>
       </c>
       <c r="E73">
-        <v>20.395199999999999</v>
+        <v>18.790600000000001</v>
       </c>
       <c r="F73">
-        <v>0.1384</v>
+        <v>0.28620000000000001</v>
       </c>
       <c r="G73">
-        <v>0.1799</v>
+        <v>2.7549000000000001</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -9177,13 +8265,13 @@
         <v>8</v>
       </c>
       <c r="E74">
-        <v>55.951999999999998</v>
+        <v>54.985199999999999</v>
       </c>
       <c r="F74">
-        <v>2.1160999999999999</v>
+        <v>2.1147999999999998</v>
       </c>
       <c r="G74">
-        <v>0.66859999999999997</v>
+        <v>0.68469999999999998</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -9200,13 +8288,13 @@
         <v>16</v>
       </c>
       <c r="E75">
-        <v>76.930599999999998</v>
+        <v>77.162099999999995</v>
       </c>
       <c r="F75">
-        <v>0.1852</v>
+        <v>0.75119999999999998</v>
       </c>
       <c r="G75">
-        <v>1.0448</v>
+        <v>0.1429</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -9223,13 +8311,13 @@
         <v>32</v>
       </c>
       <c r="E76">
-        <v>88.759399999999999</v>
+        <v>88.206299999999999</v>
       </c>
       <c r="F76">
-        <v>0.3543</v>
+        <v>5.8799999999999998E-2</v>
       </c>
       <c r="G76">
-        <v>0.24909999999999999</v>
+        <v>0.41810000000000003</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -9251,13 +8339,13 @@
         <v>2</v>
       </c>
       <c r="E79">
-        <v>27.795500000000001</v>
+        <v>27.808</v>
       </c>
       <c r="F79">
-        <v>0.19900000000000001</v>
+        <v>0.21149999999999999</v>
       </c>
       <c r="G79">
-        <v>1.2613000000000001</v>
+        <v>1.7196</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -9280,7 +8368,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
       <c r="G80">
-        <v>0.54500000000000004</v>
+        <v>1.1998</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -9303,7 +8391,7 @@
         <v>1.2070000000000001</v>
       </c>
       <c r="G81">
-        <v>0.50849999999999995</v>
+        <v>0.54369999999999996</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -9320,13 +8408,13 @@
         <v>16</v>
       </c>
       <c r="E82">
-        <v>85.440700000000007</v>
+        <v>85.621700000000004</v>
       </c>
       <c r="F82">
-        <v>0.42670000000000002</v>
+        <v>0.49320000000000003</v>
       </c>
       <c r="G82">
-        <v>0.23830000000000001</v>
+        <v>1.0669</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -9343,13 +8431,13 @@
         <v>32</v>
       </c>
       <c r="E83">
-        <v>92.389799999999994</v>
+        <v>92.349299999999999</v>
       </c>
       <c r="F83">
-        <v>0.317</v>
+        <v>0.4592</v>
       </c>
       <c r="G83">
-        <v>0.57620000000000005</v>
+        <v>9.64E-2</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -9366,13 +8454,13 @@
         <v>2</v>
       </c>
       <c r="E85">
-        <v>27.238600000000002</v>
+        <v>27.226600000000001</v>
       </c>
       <c r="F85">
-        <v>0.1812</v>
+        <v>0.86180000000000001</v>
       </c>
       <c r="G85">
-        <v>1.7083999999999999</v>
+        <v>1.7203999999999999</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -9389,13 +8477,13 @@
         <v>4</v>
       </c>
       <c r="E86">
-        <v>54.332999999999998</v>
+        <v>54.335700000000003</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="G86">
-        <v>0.43709999999999999</v>
+        <v>1.2042999999999999</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -9418,7 +8506,7 @@
         <v>1.1982999999999999</v>
       </c>
       <c r="G87">
-        <v>0.55000000000000004</v>
+        <v>0.51149999999999995</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -9435,13 +8523,13 @@
         <v>16</v>
       </c>
       <c r="E88">
-        <v>85.22</v>
+        <v>85.170900000000003</v>
       </c>
       <c r="F88">
-        <v>0.64229999999999998</v>
+        <v>0.45369999999999999</v>
       </c>
       <c r="G88">
-        <v>0.7107</v>
+        <v>0.84509999999999996</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -9458,13 +8546,13 @@
         <v>32</v>
       </c>
       <c r="E89">
-        <v>91.874799999999993</v>
+        <v>92.0565</v>
       </c>
       <c r="F89">
-        <v>1.3139000000000001</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="G89">
-        <v>0.3422</v>
+        <v>0.26929999999999998</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -9481,13 +8569,13 @@
         <v>2</v>
       </c>
       <c r="E91">
-        <v>13.2379</v>
+        <v>12.1899</v>
       </c>
       <c r="F91">
-        <v>3.0192000000000001</v>
+        <v>2.1966999999999999</v>
       </c>
       <c r="G91">
-        <v>0.32600000000000001</v>
+        <v>1.0692999999999999</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -9504,13 +8592,13 @@
         <v>4</v>
       </c>
       <c r="E92">
-        <v>35.334099999999999</v>
+        <v>34.768799999999999</v>
       </c>
       <c r="F92">
-        <v>2.5999999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="G92">
-        <v>1.6026</v>
+        <v>3.0133999999999999</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -9527,13 +8615,13 @@
         <v>8</v>
       </c>
       <c r="E93">
-        <v>59.787199999999999</v>
+        <v>59.189799999999998</v>
       </c>
       <c r="F93">
-        <v>2.8973</v>
+        <v>2.8769999999999998</v>
       </c>
       <c r="G93">
-        <v>1.2885</v>
+        <v>2.4150999999999998</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -9550,13 +8638,13 @@
         <v>16</v>
       </c>
       <c r="E94">
-        <v>76.984499999999997</v>
+        <v>76.5501</v>
       </c>
       <c r="F94">
-        <v>5.9930000000000003</v>
+        <v>0.9728</v>
       </c>
       <c r="G94">
-        <v>1.6747000000000001</v>
+        <v>1.869</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -9573,13 +8661,13 @@
         <v>32</v>
       </c>
       <c r="E95">
-        <v>87.171199999999999</v>
+        <v>87.241900000000001</v>
       </c>
       <c r="F95">
-        <v>0.22189999999999999</v>
+        <v>0.49349999999999999</v>
       </c>
       <c r="G95">
-        <v>0.92959999999999998</v>
+        <v>0.4622</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -9596,13 +8684,13 @@
         <v>2</v>
       </c>
       <c r="E97">
-        <v>1.5315000000000001</v>
+        <v>0.76670000000000005</v>
       </c>
       <c r="F97">
-        <v>1.8050999999999999</v>
+        <v>1.2616000000000001</v>
       </c>
       <c r="G97">
-        <v>9.0999999999999998E-2</v>
+        <v>0.82730000000000004</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -9619,13 +8707,13 @@
         <v>4</v>
       </c>
       <c r="E98">
-        <v>14.370100000000001</v>
+        <v>14.213800000000001</v>
       </c>
       <c r="F98">
-        <v>0.20910000000000001</v>
+        <v>0.31430000000000002</v>
       </c>
       <c r="G98">
-        <v>0.1109</v>
+        <v>2.8875000000000002</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -9642,13 +8730,13 @@
         <v>8</v>
       </c>
       <c r="E99">
-        <v>36.104799999999997</v>
+        <v>35.607900000000001</v>
       </c>
       <c r="F99">
-        <v>2.5836999999999999</v>
+        <v>2.5430999999999999</v>
       </c>
       <c r="G99">
-        <v>1.4406000000000001</v>
+        <v>1.4329000000000001</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -9665,13 +8753,13 @@
         <v>16</v>
       </c>
       <c r="E100">
-        <v>60.845999999999997</v>
+        <v>60.259399999999999</v>
       </c>
       <c r="F100">
-        <v>0.60460000000000003</v>
+        <v>0.62209999999999999</v>
       </c>
       <c r="G100">
-        <v>1.3069</v>
+        <v>0.75290000000000001</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -9688,13 +8776,13 @@
         <v>32</v>
       </c>
       <c r="E101">
-        <v>78.706000000000003</v>
+        <v>77.173000000000002</v>
       </c>
       <c r="F101">
-        <v>1.0418000000000001</v>
+        <v>0.53439999999999999</v>
       </c>
       <c r="G101">
-        <v>0.53779999999999994</v>
+        <v>1.1753</v>
       </c>
     </row>
   </sheetData>

</xml_diff>